<commit_message>
example updated due to the some changes in the src-modules
</commit_message>
<xml_diff>
--- a/examples/results_simple_analysis.xlsx
+++ b/examples/results_simple_analysis.xlsx
@@ -479,13 +479,13 @@
     </row>
     <row r="5">
       <c r="B5" s="2" t="n">
-        <v>0.3268619478386235</v>
+        <v>0.3292956137742247</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.3495541251133411</v>
+        <v>0.3623351811588255</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>0.3235839270480354</v>
+        <v>0.3083692050669497</v>
       </c>
     </row>
     <row r="7">
@@ -497,26 +497,26 @@
     </row>
     <row r="8">
       <c r="B8" s="2" t="n">
-        <v>-0.1417689256088195</v>
+        <v>-0.197038665338371</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.804094670047245</v>
+        <v>0.7923650869569785</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="2" t="n">
-        <v>-0.6254819485041706</v>
+        <v>-0.5876889617074239</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>-0.5248228260680862</v>
+        <v>-0.5668230331892988</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="2" t="n">
-        <v>0.7672508741129896</v>
+        <v>0.7847276270457945</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>-0.2792718439791587</v>
+        <v>-0.2255420537676797</v>
       </c>
     </row>
     <row r="12">
@@ -528,10 +528,10 @@
     </row>
     <row r="13">
       <c r="B13" t="n">
-        <v>0.05932596625123335</v>
+        <v>0.1003643930382884</v>
       </c>
       <c r="C13" t="n">
-        <v>0.02645774223870853</v>
+        <v>0.03913405214650325</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -563,13 +563,13 @@
     </row>
     <row r="18">
       <c r="B18" t="n">
-        <v>0.0160457924303361</v>
+        <v>0.02336250214449371</v>
       </c>
       <c r="C18" t="n">
-        <v>0.01395090153788818</v>
+        <v>0.02105042454389415</v>
       </c>
       <c r="D18" t="n">
-        <v>0.02823877022448144</v>
+        <v>0.04853158610938179</v>
       </c>
     </row>
   </sheetData>
@@ -620,13 +620,13 @@
     </row>
     <row r="5">
       <c r="B5" s="2" t="n">
-        <v>0.3910193414948027</v>
+        <v>0.3831879555466839</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.2407519774765393</v>
+        <v>0.2353965020895953</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>0.3682286810286579</v>
+        <v>0.3814155423637206</v>
       </c>
     </row>
     <row r="7">
@@ -638,26 +638,26 @@
     </row>
     <row r="8">
       <c r="B8" s="2" t="n">
-        <v>-0.7593125444893803</v>
+        <v>-0.7547402640566521</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.3001851536097842</v>
+        <v>0.3115024887193707</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="2" t="n">
-        <v>0.1196883033796828</v>
+        <v>0.107601063455275</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>-0.8076765297448973</v>
+        <v>-0.8093754862917217</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="2" t="n">
-        <v>0.6396242411096973</v>
+        <v>0.6471392006013769</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0.5074913761351127</v>
+        <v>0.49787299757235</v>
       </c>
     </row>
     <row r="12">
@@ -669,10 +669,10 @@
     </row>
     <row r="13">
       <c r="B13" t="n">
-        <v>0.1973354690421758</v>
+        <v>0.2142149150689366</v>
       </c>
       <c r="C13" t="n">
-        <v>0.09658164378649145</v>
+        <v>0.08270015596735977</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -699,10 +699,10 @@
     </row>
     <row r="18">
       <c r="B18" t="n">
-        <v>0.0932715249157081</v>
+        <v>0.09745855887588231</v>
       </c>
       <c r="C18" t="n">
-        <v>0.05578335859142281</v>
+        <v>0.05194144861041222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>